<commit_message>
Update data for generating graphs
</commit_message>
<xml_diff>
--- a/data/globaltemps/data/arcticseaice.xlsx
+++ b/data/globaltemps/data/arcticseaice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erica\Documents\Aptech\marketing\linkbuilding\globaltemps\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclow\Documents\GitHub\gauss-climatestudy\data\globaltemps\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59DE14D9-9843-49E7-B778-8ED0BF68AF21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86F8B9F-861D-484D-8CE8-F15356814E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arcticseaice" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>mo</t>
-  </si>
-  <si>
-    <t>data-type</t>
   </si>
   <si>
     <t>region</t>
@@ -48,11 +45,14 @@
   <si>
     <t>NRTSI-G</t>
   </si>
+  <si>
+    <t>datatype</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,10 +886,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -901,16 +903,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>7.05</v>
@@ -941,10 +943,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>7.67</v>
@@ -961,10 +963,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>7.14</v>
@@ -981,10 +983,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>7.3</v>
@@ -1001,10 +1003,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>7.39</v>
@@ -1021,10 +1023,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>6.81</v>
@@ -1041,10 +1043,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>6.7</v>
@@ -1061,10 +1063,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>7.41</v>
@@ -1081,10 +1083,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>7.28</v>
@@ -1101,10 +1103,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>7.37</v>
@@ -1121,10 +1123,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>7.01</v>
@@ -1141,10 +1143,10 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>6.14</v>
@@ -1161,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>6.47</v>
@@ -1181,10 +1183,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>7.47</v>
@@ -1201,10 +1203,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>6.4</v>
@@ -1221,10 +1223,10 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>7.14</v>
@@ -1241,10 +1243,10 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <v>6.08</v>
@@ -1261,10 +1263,10 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>7.58</v>
@@ -1281,10 +1283,10 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20">
         <v>6.69</v>
@@ -1301,10 +1303,10 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <v>6.54</v>
@@ -1321,10 +1323,10 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22">
         <v>6.12</v>
@@ -1341,10 +1343,10 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <v>6.25</v>
@@ -1361,10 +1363,10 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24">
         <v>6.73</v>
@@ -1381,10 +1383,10 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>5.83</v>
@@ -1401,10 +1403,10 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <v>6.12</v>
@@ -1421,10 +1423,10 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27">
         <v>5.98</v>
@@ -1441,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>5.5</v>
@@ -1461,10 +1463,10 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>5.86</v>
@@ -1481,10 +1483,10 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30">
         <v>4.2699999999999996</v>
@@ -1501,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31">
         <v>4.6900000000000004</v>
@@ -1521,10 +1523,10 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>5.26</v>
@@ -1541,10 +1543,10 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>4.87</v>
@@ -1561,10 +1563,10 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <v>4.5599999999999996</v>
@@ -1581,10 +1583,10 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>3.57</v>
@@ -1601,10 +1603,10 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36">
         <v>5.21</v>
@@ -1621,10 +1623,10 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>5.22</v>
@@ -1641,10 +1643,10 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38">
         <v>4.62</v>
@@ -1661,10 +1663,10 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>4.53</v>
@@ -1681,10 +1683,10 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40">
         <v>4.82</v>
@@ -1701,10 +1703,10 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <v>4.79</v>
@@ -1721,10 +1723,10 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42">
         <v>4.32</v>

</xml_diff>